<commit_message>
up import lenses & stock & product
</commit_message>
<xml_diff>
--- a/public/sample_files/add_stock_import.xlsx
+++ b/public/sample_files/add_stock_import.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xamp7_4\htdocs\pos-online\public\sample_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04405815-5DA7-44C0-BF23-556BD2EE0540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="add_stock_import" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>product_code</t>
   </si>
@@ -33,29 +27,14 @@
   <si>
     <t>sell_price</t>
   </si>
-  <si>
-    <t>batch_number</t>
-  </si>
-  <si>
-    <t>manufacturing_date</t>
-  </si>
-  <si>
-    <t>expiry_date</t>
-  </si>
-  <si>
-    <t>expiry_warning</t>
-  </si>
-  <si>
-    <t>convert_status_expire</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -537,7 +516,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -851,24 +830,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
@@ -878,7 +857,7 @@
     <col min="9" max="9" width="21" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -891,23 +870,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4324234</v>
       </c>
@@ -920,23 +884,8 @@
       <c r="D2">
         <v>200</v>
       </c>
-      <c r="E2">
-        <v>54546</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45134</v>
-      </c>
-      <c r="G2" s="2">
-        <v>45134</v>
-      </c>
-      <c r="H2" s="1">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>21321312</v>
       </c>
@@ -948,21 +897,6 @@
       </c>
       <c r="D3">
         <v>200</v>
-      </c>
-      <c r="E3">
-        <v>4324234</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45135</v>
-      </c>
-      <c r="G3" s="2">
-        <v>45134</v>
-      </c>
-      <c r="H3" s="1">
-        <v>5</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>